<commit_message>
filter search by year
</commit_message>
<xml_diff>
--- a/card_data/B/Languedoc.xlsx
+++ b/card_data/B/Languedoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alyssa/Documents/GitHub/playing-cards/backend/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryaanahmed\dev\french-playing-cards\card_data\B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EFC337-10B2-4F47-B94D-B34BFCF6C25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F11F45-F6AF-4D14-9173-E2B3A38F859E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="540" windowWidth="15760" windowHeight="16420" xr2:uid="{10303BB8-D5C4-BD4D-90E9-B8596F512034}"/>
+    <workbookView xWindow="7343" yWindow="540" windowWidth="15758" windowHeight="16418" xr2:uid="{10303BB8-D5C4-BD4D-90E9-B8596F512034}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
   <si>
     <t>DB ID</t>
   </si>
@@ -178,6 +169,12 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t>Languedoc.QC.1</t>
+  </si>
+  <si>
+    <t>Languedoc.QC.2</t>
   </si>
 </sst>
 </file>
@@ -539,23 +536,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31051152-4AC0-9644-9460-F5BBAE33FC46}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.3125" customWidth="1"/>
+    <col min="2" max="2" width="13.6875" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.8125" customWidth="1"/>
+    <col min="5" max="5" width="10.3125" customWidth="1"/>
+    <col min="11" max="11" width="18.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -628,7 +625,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -663,7 +660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -698,7 +695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -733,7 +730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -768,7 +765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -803,7 +800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -838,7 +835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -873,7 +870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -908,7 +905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -943,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -978,7 +975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1013,7 +1010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1083,7 +1080,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1188,7 +1185,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1258,7 +1255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1293,7 +1290,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1328,7 +1325,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1360,6 +1357,76 @@
         <v>13</v>
       </c>
       <c r="L23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>1702</v>
+      </c>
+      <c r="G24">
+        <v>1720</v>
+      </c>
+      <c r="I24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" t="s">
+        <v>45</v>
+      </c>
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <v>1702</v>
+      </c>
+      <c r="G25">
+        <v>1720</v>
+      </c>
+      <c r="I25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>